<commit_message>
updated block foil count, cleaning
</commit_message>
<xml_diff>
--- a/data/sub-9999/retrieval4.xlsx
+++ b/data/sub-9999/retrieval4.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="102">
   <si>
     <t>retrieval4</t>
   </si>
@@ -275,6 +275,42 @@
   </si>
   <si>
     <t>SetD/072a.jpg</t>
+  </si>
+  <si>
+    <t>SetD/073a.jpg</t>
+  </si>
+  <si>
+    <t>SetD/074a.jpg</t>
+  </si>
+  <si>
+    <t>SetD/075a.jpg</t>
+  </si>
+  <si>
+    <t>SetD/076a.jpg</t>
+  </si>
+  <si>
+    <t>SetD/077a.jpg</t>
+  </si>
+  <si>
+    <t>SetD/078a.jpg</t>
+  </si>
+  <si>
+    <t>SetD/079a.jpg</t>
+  </si>
+  <si>
+    <t>SetD/080a.jpg</t>
+  </si>
+  <si>
+    <t>SetD/081a.jpg</t>
+  </si>
+  <si>
+    <t>SetD/082a.jpg</t>
+  </si>
+  <si>
+    <t>SetD/083a.jpg</t>
+  </si>
+  <si>
+    <t>SetD/084a.jpg</t>
   </si>
   <si>
     <t>targ</t>
@@ -641,7 +677,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -663,7 +699,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -674,7 +710,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -685,7 +721,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -696,7 +732,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -707,7 +743,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -718,7 +754,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -729,7 +765,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -740,7 +776,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -751,7 +787,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -762,7 +798,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -773,7 +809,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -784,7 +820,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -795,7 +831,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -806,7 +842,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -817,7 +853,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -828,7 +864,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -839,7 +875,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -850,7 +886,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -861,7 +897,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -872,7 +908,7 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -883,7 +919,7 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -894,7 +930,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -905,7 +941,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -916,7 +952,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -927,7 +963,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -938,7 +974,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -949,7 +985,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -960,7 +996,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -971,7 +1007,7 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -982,7 +1018,7 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -993,7 +1029,7 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -1004,7 +1040,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -1015,7 +1051,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -1026,7 +1062,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -1037,7 +1073,7 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -1048,7 +1084,7 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -1059,7 +1095,7 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -1070,7 +1106,7 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C39">
         <v>2</v>
@@ -1081,7 +1117,7 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -1092,7 +1128,7 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -1103,7 +1139,7 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C42">
         <v>2</v>
@@ -1114,7 +1150,7 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -1125,7 +1161,7 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C44">
         <v>2</v>
@@ -1136,7 +1172,7 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -1147,7 +1183,7 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C46">
         <v>2</v>
@@ -1158,7 +1194,7 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C47">
         <v>2</v>
@@ -1169,7 +1205,7 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C48">
         <v>2</v>
@@ -1180,7 +1216,7 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C49">
         <v>2</v>
@@ -1191,7 +1227,7 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -1202,7 +1238,7 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C51">
         <v>3</v>
@@ -1213,7 +1249,7 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C52">
         <v>3</v>
@@ -1224,7 +1260,7 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C53">
         <v>3</v>
@@ -1235,7 +1271,7 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C54">
         <v>3</v>
@@ -1246,7 +1282,7 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C55">
         <v>3</v>
@@ -1257,7 +1293,7 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C56">
         <v>3</v>
@@ -1268,7 +1304,7 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C57">
         <v>3</v>
@@ -1279,7 +1315,7 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C58">
         <v>3</v>
@@ -1290,7 +1326,7 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C59">
         <v>3</v>
@@ -1301,7 +1337,7 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C60">
         <v>3</v>
@@ -1312,7 +1348,7 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C61">
         <v>3</v>
@@ -1323,7 +1359,7 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C62">
         <v>3</v>
@@ -1334,7 +1370,7 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C63">
         <v>3</v>
@@ -1345,7 +1381,7 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C64">
         <v>3</v>
@@ -1356,7 +1392,7 @@
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C65">
         <v>3</v>
@@ -1367,7 +1403,7 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C66">
         <v>3</v>
@@ -1378,7 +1414,7 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C67">
         <v>3</v>
@@ -1389,7 +1425,7 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C68">
         <v>3</v>
@@ -1400,7 +1436,7 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C69">
         <v>3</v>
@@ -1411,7 +1447,7 @@
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C70">
         <v>3</v>
@@ -1422,7 +1458,7 @@
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C71">
         <v>3</v>
@@ -1433,7 +1469,7 @@
         <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C72">
         <v>3</v>
@@ -1444,7 +1480,7 @@
         <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C73">
         <v>3</v>
@@ -1455,7 +1491,7 @@
         <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C74">
         <v>3</v>
@@ -1466,7 +1502,7 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C75">
         <v>3</v>
@@ -1477,7 +1513,7 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C76">
         <v>3</v>
@@ -1488,7 +1524,7 @@
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C77">
         <v>3</v>
@@ -1499,7 +1535,7 @@
         <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C78">
         <v>3</v>
@@ -1510,7 +1546,7 @@
         <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C79">
         <v>3</v>
@@ -1521,7 +1557,7 @@
         <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C80">
         <v>3</v>
@@ -1532,7 +1568,7 @@
         <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C81">
         <v>3</v>
@@ -1543,7 +1579,7 @@
         <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C82">
         <v>3</v>
@@ -1554,7 +1590,7 @@
         <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C83">
         <v>3</v>
@@ -1565,7 +1601,7 @@
         <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C84">
         <v>3</v>
@@ -1576,9 +1612,141 @@
         <v>86</v>
       </c>
       <c r="B85" t="s">
+        <v>101</v>
+      </c>
+      <c r="C85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" t="s">
+        <v>101</v>
+      </c>
+      <c r="C86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
+      <c r="B87" t="s">
+        <v>101</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
         <v>89</v>
       </c>
-      <c r="C85">
+      <c r="B88" t="s">
+        <v>101</v>
+      </c>
+      <c r="C88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89" t="s">
+        <v>101</v>
+      </c>
+      <c r="C89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90" t="s">
+        <v>101</v>
+      </c>
+      <c r="C90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91" t="s">
+        <v>101</v>
+      </c>
+      <c r="C91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>93</v>
+      </c>
+      <c r="B92" t="s">
+        <v>101</v>
+      </c>
+      <c r="C92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>94</v>
+      </c>
+      <c r="B93" t="s">
+        <v>101</v>
+      </c>
+      <c r="C93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>95</v>
+      </c>
+      <c r="B94" t="s">
+        <v>101</v>
+      </c>
+      <c r="C94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>96</v>
+      </c>
+      <c r="B95" t="s">
+        <v>101</v>
+      </c>
+      <c r="C95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>97</v>
+      </c>
+      <c r="B96" t="s">
+        <v>101</v>
+      </c>
+      <c r="C96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>98</v>
+      </c>
+      <c r="B97" t="s">
+        <v>101</v>
+      </c>
+      <c r="C97">
         <v>3</v>
       </c>
     </row>

</xml_diff>